<commit_message>
Added .zip of gerbers. Fixed minor issues with assembly files.
</commit_message>
<xml_diff>
--- a/v0p2/gerber_v0p2_r1/BOM_JLCPCB.xlsx
+++ b/v0p2/gerber_v0p2_r1/BOM_JLCPCB.xlsx
@@ -86,7 +86,7 @@
     <t xml:space="preserve">C1, C3     </t>
   </si>
   <si>
-    <t xml:space="preserve">  C15849     </t>
+    <t xml:space="preserve">C15849     </t>
   </si>
   <si>
     <t xml:space="preserve">0.1uF ceramic capacitor  </t>
@@ -95,7 +95,7 @@
     <t xml:space="preserve">C2        </t>
   </si>
   <si>
-    <t xml:space="preserve">  C14663     </t>
+    <t xml:space="preserve">C14663     </t>
   </si>
   <si>
     <t xml:space="preserve">10k resistor 0.1%        </t>
@@ -104,7 +104,7 @@
     <t xml:space="preserve">R1, R2, R3  </t>
   </si>
   <si>
-    <t xml:space="preserve">  C190321    </t>
+    <t xml:space="preserve">C190321    </t>
   </si>
   <si>
     <t xml:space="preserve">4.7k resistor 1%         </t>
@@ -113,7 +113,7 @@
     <t xml:space="preserve">R4        </t>
   </si>
   <si>
-    <t xml:space="preserve">  C23162     </t>
+    <t xml:space="preserve">C23162     </t>
   </si>
   <si>
     <t xml:space="preserve">switch SPST-NO           </t>
@@ -125,7 +125,7 @@
     <t xml:space="preserve">    SW-SMD-2_2.9x3.9x1.7  </t>
   </si>
   <si>
-    <t xml:space="preserve">  C115357    </t>
+    <t xml:space="preserve">C115357    </t>
   </si>
   <si>
     <t xml:space="preserve">MCP6002T-I/SN opamp      </t>
@@ -137,7 +137,7 @@
     <t xml:space="preserve">    SOIC-8_3.9x4.9x1.27P  </t>
   </si>
   <si>
-    <t xml:space="preserve">  C7377      </t>
+    <t xml:space="preserve">C7377      </t>
   </si>
 </sst>
 </file>
@@ -368,7 +368,7 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>